<commit_message>
Change to allowable values Terminal_inventory argument of cmdty.CreateStorage function and addition of associated Terminal_val_param argument.
</commit_message>
<xml_diff>
--- a/samples/excel/three_factor_storage.xlsx
+++ b/samples/excel/three_factor_storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\source\repos\storage\samples\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401332E9-0278-40AC-946B-EB23C664147E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C25602-D016-4CE4-9DF9-0EA4C65C59C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="585" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="553" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add-in Info" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <definedName name="StorageObject">Storage!$C$2</definedName>
     <definedName name="ValDate">Storage!$S$6</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>Inject/Withdraw/Inventory Constraints</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Terminal Inventory</t>
   </si>
   <si>
-    <t>ZeroValue</t>
-  </si>
-  <si>
     <t>Add-in Version</t>
   </si>
   <si>
@@ -279,6 +276,12 @@
   </si>
   <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Terminal inventory Param</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,13 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -421,68 +430,82 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv_a9187915a6754976b0d4807fa550e135">
+    <main first="rtdsrv_eeee467a459e4b58bf6fcb873cfb4382">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>b6210142-bf76-4333-bc04-f5bfe4f5e93b</stp>
-        <tr r="AE8" s="1"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>7ae1c4d1-cc34-4515-95ae-f57a989c7887</stp>
+        <stp>807cbd47-9f43-48db-a522-039536abbc4b</stp>
         <tr r="BC16" s="1"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>64641cbc-c69f-4f20-9a8f-7ea4d9a9b08e</stp>
-        <tr r="AE11" s="1"/>
+        <stp>4934b6da-4c01-43ae-9710-5b2405899c74</stp>
+        <tr r="AE8" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv_a9187915a6754976b0d4807fa550e135">
+    <main first="rtdsrv_eeee467a459e4b58bf6fcb873cfb4382">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>a617131d-bb7f-42fe-be25-a8e0b3d806f4</stp>
-        <tr r="AD16" s="1"/>
+        <stp>de5fea1e-7803-404d-892e-7b304ce7c04c</stp>
+        <tr r="AE4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_eeee467a459e4b58bf6fcb873cfb4382">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>9857ba4b-8866-40b9-9775-d37ed586fe07</stp>
+        <tr r="AE11" s="1"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>ef0702e9-f43c-4233-936e-594525466206</stp>
+        <stp>15ace416-d622-4ff9-a001-fe0992a1e1fd</stp>
+        <tr r="C2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_eeee467a459e4b58bf6fcb873cfb4382">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>e847976c-d41e-4b0c-b059-610e555fd177</stp>
+        <tr r="AE6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_eeee467a459e4b58bf6fcb873cfb4382">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>8c89a826-cc95-470d-b73f-fc5f06df6223</stp>
         <tr r="AE7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_eeee467a459e4b58bf6fcb873cfb4382">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>0f4ac8c3-f857-4c67-86db-e76dd6f69c77</stp>
+        <tr r="AG16" s="1"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>eb8c672f-feb7-46ad-b724-4e8851881894</stp>
-        <tr r="AE6" s="1"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>4a16bd20-633a-4a1c-8ef8-210ae6f9387f</stp>
-        <tr r="AE4" s="1"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>8530cf8b-a9ab-42da-aafe-1a2524197dbc</stp>
-        <tr r="C2" s="1"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>ff95ed0a-cdc4-4392-94d3-99f678807535</stp>
+        <stp>be0c9b12-bfc4-42eb-b50b-edffde8830ac</stp>
         <tr r="AM16" s="1"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>6351ff81-e5ab-4795-b1e0-25d6b47ddcdc</stp>
-        <tr r="AG16" s="1"/>
+        <stp>852aa2dc-ea69-42f9-aa90-dca733978695</stp>
+        <tr r="AE9" s="1"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>251c20d3-305d-4d98-acde-efad28a260e2</stp>
+        <tr r="AD16" s="1"/>
       </tp>
     </main>
   </volType>
@@ -1501,7 +1524,7 @@
                   <c:v>18000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3177,7 +3200,7 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="12" t="str" cm="1">
         <f t="array" ref="C3">_xll.cmdty.StorageAddInVersion()</f>
@@ -3186,7 +3209,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="12" t="str" cm="1">
         <f t="array" ref="C4">_xll.cmdty.LinearAlgebraProvider()</f>
@@ -3201,16 +3224,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:BD2391"/>
+  <dimension ref="B2:BD2391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE10" sqref="AE10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
@@ -3234,35 +3257,29 @@
     <col min="55" max="55" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:56" x14ac:dyDescent="0.25">
-      <c r="C1" t="str">
-        <f>C2</f>
-        <v>storage:2</v>
-      </c>
-    </row>
     <row r="2" spans="2:56" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C2" s="12" t="str" cm="1">
-        <f t="array" ref="C2">_xll.cmdty.CreateStorage(B2,C6,C7,E6:H291,F3,C10,C11,C14,C15,C17)</f>
-        <v>storage:2</v>
+        <f t="array" ref="C2">_xll.cmdty.CreateStorage(B2,C6,C7,E6:H291,F3,C10,C11,C14,C15,C17,C18)</f>
+        <v>storage:18</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>53</v>
       </c>
       <c r="AE2" cm="1">
         <f t="array" aca="1" ref="AE2" ca="1">_xll.cmdty.NumberOfRunningCalculations()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:56" x14ac:dyDescent="0.25">
@@ -3290,11 +3307,11 @@
         <v>31</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AE4" s="12" t="str" cm="1">
         <f t="array" ref="AE4">_xll.cmdty.StorageIntrinsicValue(AD4,StorageObject,ValDate,Inventory,MktData.FwdCurve,MktData.IrCurve,StaticData.SettleDates, McParams.GridPoints, McParams.NumTol)</f>
-        <v>Intrinsic Value:3</v>
+        <v>Intrinsic Value:19</v>
       </c>
     </row>
     <row r="5" spans="2:56" x14ac:dyDescent="0.25">
@@ -3323,10 +3340,10 @@
         <v>3</v>
       </c>
       <c r="O5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>3</v>
@@ -3418,7 +3435,7 @@
       </c>
       <c r="AE6" s="12" t="str" cm="1">
         <f t="array" ref="AE6">_xll.cmdty.StorageValueThreeFactor(AD6, C2, S6,S7,AA6:AB2391, U6:V99,S11,S12,S13,S14,S8,'Static Data'!B4:C145, McParams.NumSims, McParams.BasisFuncs, McParams.Seed, McParams.FwdSeed, McParams.GridPoints, McParams.NumTol, McParams.ExtraDecs)</f>
-        <v>3-factor val:4</v>
+        <v>3-factor val:20</v>
       </c>
     </row>
     <row r="7" spans="2:56" x14ac:dyDescent="0.25">
@@ -3495,7 +3512,7 @@
       </c>
       <c r="AE7" t="str" cm="1">
         <f t="array" ref="AE7">_xll.cmdty.SubscribeStatus(AE6)</f>
-        <v>Cancelled</v>
+        <v>Running</v>
       </c>
     </row>
     <row r="8" spans="2:56" x14ac:dyDescent="0.25">
@@ -3566,7 +3583,7 @@
       </c>
       <c r="AE8" s="18" cm="1">
         <f t="array" ref="AE8">_xll.cmdty.SubscribeProgress(AE6)</f>
-        <v>0.85586324786325652</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3630,7 +3647,7 @@
         <v>54</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE9" t="e" cm="1">
         <f t="array" ref="AE9">_xll.cmdty.SubscribeError(Results.ThreeFactorVal)</f>
@@ -3845,7 +3862,7 @@
         <v>54</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE12" s="17" cm="1">
         <f t="array" ref="AE12">_xll.cmdty.GetObjectProperty(Results.IntrinsicVal, "Npv")</f>
@@ -3915,7 +3932,7 @@
         <v>52.68</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE13" s="17" t="e">
         <f>AE11-AE12</f>
@@ -3994,10 +4011,10 @@
         <v>41</v>
       </c>
       <c r="AU14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AV14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4223,7 +4240,7 @@
         <v>54</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E17" s="7">
         <v>43815</v>
@@ -4316,6 +4333,10 @@
       <c r="BD17" s="23"/>
     </row>
     <row r="18" spans="2:56" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="2"/>
       <c r="E18" s="7">
         <v>43815</v>
       </c>
@@ -4341,7 +4362,7 @@
       </c>
       <c r="P18" s="24" cm="1">
         <f t="array" ref="P18">_xll.cmdty.StorageMaxInventory(StorageObject,N18)</f>
-        <v>18000</v>
+        <v>0</v>
       </c>
       <c r="U18" s="3"/>
       <c r="V18" s="16"/>
@@ -51216,7 +51237,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AE8">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -51229,7 +51250,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="3">
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$C$17="Empty"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8" xr:uid="{851CFE34-DBF7-4E8E-8342-553973F79B04}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
@@ -51237,7 +51263,7 @@
       <formula1>"PiecewiseLinear,Step,Polynomial"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{0C55FB1B-2BA9-43C3-8784-7B11BA3534FF}">
-      <formula1>"Empty,ZeroValue,SpotValue"</formula1>
+      <formula1>"Empty,SpotValueMultiple,InventoryMultiple"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>